<commit_message>
Anonymisation des bulletins exemples
</commit_message>
<xml_diff>
--- a/resources/bulletin.xlsx
+++ b/resources/bulletin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive\Bureau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\PycharmProjects\projetM1\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BA06F50-1248-4D1A-9093-E68F346D6C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FCF9A97-C366-41A0-8D70-48E309CB1CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="-120" windowWidth="27915" windowHeight="16440" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="9" xr2:uid="{141C5681-F0FA-4520-A894-4EC8430921ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Nom" sheetId="1" r:id="rId1"/>
@@ -41,54 +41,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="90">
   <si>
     <t>4TT</t>
-  </si>
-  <si>
-    <t>Jade</t>
-  </si>
-  <si>
-    <t>Emilien</t>
-  </si>
-  <si>
-    <t>Logan</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>Asenga</t>
-  </si>
-  <si>
-    <t>Angélina</t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
-    <t>Isalyne</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>Chloé</t>
-  </si>
-  <si>
-    <t>Hérésia</t>
-  </si>
-  <si>
-    <t>Keurtys</t>
-  </si>
-  <si>
-    <t>Clhéo</t>
-  </si>
-  <si>
-    <t>Camille</t>
-  </si>
-  <si>
-    <t>Emma</t>
-  </si>
-  <si>
-    <t>Basile</t>
   </si>
   <si>
     <t>U1 – Music database + voc p15 10/09</t>
@@ -333,15 +285,64 @@
   <si>
     <t>% Juin</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1288,7 +1289,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -1313,23 +1314,23 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1353,7 +1354,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Rouge" xfId="1"/>
+    <cellStyle name="Rouge" xfId="1" xr:uid="{49156F99-B74F-4BBE-8C8E-F7C30537138D}"/>
   </cellStyles>
   <dxfs count="30">
     <dxf>
@@ -2058,10 +2059,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C268F7-A06D-4CC6-86A2-06B81193E202}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2089,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2097,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2105,7 +2108,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2113,7 +2116,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2121,7 +2124,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2129,7 +2132,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2137,7 +2140,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2145,7 +2148,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2153,7 +2156,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2161,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2169,7 +2172,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2177,7 +2180,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2185,7 +2188,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2193,7 +2196,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2201,7 +2204,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2209,7 +2212,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2295,7 +2298,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1AC9C3-9F15-4089-82AB-04371078902F}">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -2315,44 +2318,44 @@
   <sheetData>
     <row r="1" spans="1:16" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="98" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="7" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2419,7 +2422,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="87">
         <f>'B1'!X4</f>
@@ -2477,7 +2480,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="87">
         <f>'B1'!X5</f>
@@ -2536,7 +2539,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="87">
         <f>'B1'!X6</f>
@@ -2595,7 +2598,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="87">
         <f>'B1'!X7</f>
@@ -2654,7 +2657,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="87">
         <f>'B1'!X8</f>
@@ -2713,7 +2716,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="87">
         <f>'B1'!X9</f>
@@ -2772,7 +2775,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="87">
         <f>'B1'!X10</f>
@@ -2831,7 +2834,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="87">
         <f>'B1'!X11</f>
@@ -2890,7 +2893,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="87">
         <f>'B1'!X12</f>
@@ -2949,7 +2952,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="87">
         <f>'B1'!X13</f>
@@ -3008,7 +3011,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="87">
         <f>'B1'!X14</f>
@@ -3067,7 +3070,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="87">
         <f>'B1'!X15</f>
@@ -3126,7 +3129,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="87">
         <f>'B1'!X16</f>
@@ -3185,7 +3188,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="87">
         <f>'B1'!X17</f>
@@ -3244,7 +3247,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="87">
         <f>'B1'!X18</f>
@@ -3303,7 +3306,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="87">
         <f>'B1'!X19</f>
@@ -3994,7 +3997,7 @@
     </row>
     <row r="31" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59">
         <f t="shared" ref="C31:N31" si="6">AVERAGE(C4:C19)</f>
@@ -4060,7 +4063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875FBB08-23D3-4311-8DC8-F019AE017944}">
   <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -4104,25 +4107,25 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="AA1" s="1"/>
@@ -4172,14 +4175,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -4214,34 +4217,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4250,7 +4253,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="34"/>
       <c r="D4" s="35"/>
@@ -4345,7 +4348,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="49"/>
       <c r="D5" s="50"/>
@@ -4440,7 +4443,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="50"/>
@@ -4535,7 +4538,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="50"/>
@@ -4630,7 +4633,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="50"/>
@@ -4725,7 +4728,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="49"/>
       <c r="D9" s="50"/>
@@ -4820,7 +4823,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="49"/>
       <c r="D10" s="50"/>
@@ -4915,7 +4918,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="49"/>
       <c r="D11" s="50"/>
@@ -5010,7 +5013,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="49"/>
       <c r="D12" s="50"/>
@@ -5105,7 +5108,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="49"/>
       <c r="D13" s="50"/>
@@ -5200,7 +5203,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="49"/>
       <c r="D14" s="50"/>
@@ -5295,7 +5298,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="49"/>
       <c r="D15" s="50"/>
@@ -5390,7 +5393,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="50"/>
@@ -5485,7 +5488,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="49"/>
       <c r="D17" s="50"/>
@@ -5580,7 +5583,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="50"/>
@@ -5675,7 +5678,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="49"/>
       <c r="D19" s="50"/>
@@ -6810,7 +6813,7 @@
     </row>
     <row r="31" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59" t="e">
         <f t="shared" ref="C31:X31" si="18">AVERAGE(C4:C30)</f>
@@ -6923,7 +6926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D987A1A4-4A1A-45D8-811D-D5A859BE3C1E}">
   <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -6953,31 +6956,31 @@
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="7" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -6986,29 +6989,29 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -7076,14 +7079,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -7094,31 +7097,31 @@
       <c r="A3" s="95"/>
       <c r="B3" s="95"/>
       <c r="C3" s="22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
@@ -7136,34 +7139,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7172,7 +7175,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="31">
         <v>4</v>
@@ -7284,7 +7287,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="46">
         <v>8.5</v>
@@ -7396,7 +7399,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="46">
         <v>4.5</v>
@@ -7508,7 +7511,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="47"/>
@@ -7620,7 +7623,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="46">
         <v>5.5</v>
@@ -7732,7 +7735,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="46">
         <v>7.5</v>
@@ -7844,7 +7847,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="46">
         <v>7.5</v>
@@ -7956,7 +7959,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="46">
         <v>6</v>
@@ -8068,7 +8071,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="46">
         <v>9.5</v>
@@ -8180,7 +8183,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="46">
         <v>8</v>
@@ -8292,7 +8295,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="46">
         <v>10.5</v>
@@ -8404,7 +8407,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="46"/>
       <c r="D15" s="47"/>
@@ -8516,7 +8519,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="46">
         <v>7</v>
@@ -8628,7 +8631,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="46">
         <v>6</v>
@@ -8740,7 +8743,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="46">
         <v>11</v>
@@ -8852,7 +8855,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="46"/>
       <c r="D19" s="47"/>
@@ -10023,7 +10026,7 @@
     </row>
     <row r="31" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59">
         <f t="shared" ref="C31:I31" si="21">AVERAGE(C4:C18)</f>
@@ -10116,19 +10119,19 @@
     </row>
     <row r="33" spans="18:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R33" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S33" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="T33" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="V33" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -10147,7 +10150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDA5899-4D9E-4F70-BF8E-9B5A21969541}">
   <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -10176,25 +10179,25 @@
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
@@ -10205,29 +10208,29 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -10291,14 +10294,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -10309,25 +10312,25 @@
       <c r="A3" s="95"/>
       <c r="B3" s="95"/>
       <c r="C3" s="22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="23"/>
@@ -10347,34 +10350,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10383,7 +10386,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="72">
         <v>3</v>
@@ -10495,7 +10498,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="74">
         <v>4</v>
@@ -10607,7 +10610,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="74">
         <v>4</v>
@@ -10719,7 +10722,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="74">
         <v>5</v>
@@ -10831,7 +10834,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="74">
         <v>4</v>
@@ -10943,7 +10946,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="74">
         <v>0</v>
@@ -11055,7 +11058,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="74">
         <v>4</v>
@@ -11167,7 +11170,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="74">
         <v>2</v>
@@ -11279,7 +11282,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="74"/>
       <c r="D12" s="51">
@@ -11385,7 +11388,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="74">
         <v>2</v>
@@ -11497,7 +11500,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="74">
         <v>0</v>
@@ -11609,7 +11612,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="74">
         <v>2</v>
@@ -11719,7 +11722,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="51">
@@ -11829,7 +11832,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="74">
         <v>0</v>
@@ -11939,7 +11942,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="74">
         <v>0</v>
@@ -12051,7 +12054,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="74"/>
       <c r="D19" s="51"/>
@@ -13226,7 +13229,7 @@
     </row>
     <row r="31" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59">
         <f>AVERAGE(C4:C18)</f>
@@ -13319,19 +13322,19 @@
     </row>
     <row r="33" spans="18:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R33" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S33" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="T33" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="V33" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -13370,10 +13373,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260BB258-8DE8-41D2-8C03-28BCFB82D200}">
   <dimension ref="A1:AJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
@@ -13394,74 +13397,74 @@
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="7" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -13541,14 +13544,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -13559,49 +13562,49 @@
       <c r="A3" s="95"/>
       <c r="B3" s="95"/>
       <c r="C3" s="22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="L3" s="22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="R3" s="25"/>
       <c r="S3" s="25"/>
@@ -13613,34 +13616,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
@@ -13649,7 +13652,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="31">
         <v>4</v>
@@ -13770,7 +13773,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="46">
         <v>8.5</v>
@@ -13891,7 +13894,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="46">
         <v>4.5</v>
@@ -14012,7 +14015,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="47"/>
@@ -14133,7 +14136,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="46">
         <v>5.5</v>
@@ -14254,7 +14257,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="46">
         <v>7.5</v>
@@ -14375,7 +14378,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="46">
         <v>7.5</v>
@@ -14496,7 +14499,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="46">
         <v>6</v>
@@ -14617,7 +14620,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="46">
         <v>9.5</v>
@@ -14732,7 +14735,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="46">
         <v>8</v>
@@ -14853,7 +14856,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="46">
         <v>10.5</v>
@@ -14974,7 +14977,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="46"/>
       <c r="D15" s="47"/>
@@ -15093,7 +15096,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="46">
         <v>7</v>
@@ -15212,7 +15215,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="46">
         <v>6</v>
@@ -15331,7 +15334,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="46">
         <v>11</v>
@@ -15452,7 +15455,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="46"/>
       <c r="D19" s="47"/>
@@ -16627,7 +16630,7 @@
     </row>
     <row r="31" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59">
         <f t="shared" ref="C31:X31" si="19">AVERAGE(C4:C19)</f>
@@ -16720,19 +16723,19 @@
     </row>
     <row r="33" spans="18:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R33" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S33" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="T33" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="V33" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -16772,7 +16775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377CC0D2-9395-4100-8A80-221F3FD3C332}">
   <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -16801,10 +16804,10 @@
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="7" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E1" s="80">
         <v>44540</v>
@@ -16824,29 +16827,29 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -16904,14 +16907,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -16922,16 +16925,16 @@
       <c r="A3" s="95"/>
       <c r="B3" s="95"/>
       <c r="C3" s="22" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -16954,34 +16957,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -16990,7 +16993,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="34">
         <v>3</v>
@@ -17096,7 +17099,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="49">
         <v>7.5</v>
@@ -17202,7 +17205,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="49">
         <v>9</v>
@@ -17308,7 +17311,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="49">
         <v>10.6</v>
@@ -17414,7 +17417,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="49">
         <v>10.9</v>
@@ -17520,7 +17523,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="49">
         <v>6.9</v>
@@ -17626,7 +17629,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="49">
         <v>8.6999999999999993</v>
@@ -17732,7 +17735,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="49">
         <v>9.6</v>
@@ -17838,7 +17841,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="49">
         <v>15.7</v>
@@ -17944,7 +17947,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="49">
         <v>12.7</v>
@@ -18050,7 +18053,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="49">
         <v>6.9</v>
@@ -18156,7 +18159,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="49">
         <v>11.8</v>
@@ -18262,7 +18265,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="49">
         <v>9</v>
@@ -18368,7 +18371,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="49">
         <v>4.2</v>
@@ -18474,7 +18477,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="49">
         <v>11.8</v>
@@ -18580,7 +18583,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="49">
         <v>11.2</v>
@@ -19759,7 +19762,7 @@
     </row>
     <row r="31" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59">
         <f t="shared" ref="C31:X31" si="21">AVERAGE(C4:C19)</f>
@@ -19852,19 +19855,19 @@
     </row>
     <row r="33" spans="18:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R33" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="S33" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="T33" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="V33" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -19903,7 +19906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218FB9B2-2FEC-4B31-BFD5-6D73CFBD7F21}">
   <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -19932,28 +19935,28 @@
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="7" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -19963,29 +19966,29 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -20051,14 +20054,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -20069,28 +20072,28 @@
       <c r="A3" s="95"/>
       <c r="B3" s="95"/>
       <c r="C3" s="22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
@@ -20109,34 +20112,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -20145,7 +20148,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="34">
         <v>5.5</v>
@@ -20259,7 +20262,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="49">
         <v>8</v>
@@ -20373,7 +20376,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="49">
         <v>7</v>
@@ -20483,7 +20486,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="49">
         <v>2</v>
@@ -20597,7 +20600,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="49">
         <v>5.5</v>
@@ -20711,7 +20714,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="49">
         <v>5</v>
@@ -20825,7 +20828,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="49">
         <v>6</v>
@@ -20939,7 +20942,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="49">
         <v>5.5</v>
@@ -21053,7 +21056,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="49">
         <v>8</v>
@@ -21165,7 +21168,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="49">
         <v>7</v>
@@ -21277,7 +21280,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="49">
         <v>4</v>
@@ -21389,7 +21392,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="49">
         <v>7</v>
@@ -21503,7 +21506,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="49">
         <v>4.5</v>
@@ -21615,7 +21618,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="49">
         <v>5.5</v>
@@ -21725,7 +21728,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="49">
         <v>5</v>
@@ -21835,7 +21838,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="49">
         <v>6.5</v>
@@ -23018,7 +23021,7 @@
     </row>
     <row r="31" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59">
         <f t="shared" ref="C31:J31" si="20">AVERAGE(C4:C19)</f>
@@ -23111,19 +23114,19 @@
     </row>
     <row r="33" spans="18:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R33" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S33" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="T33" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="V33" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -23162,7 +23165,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72AADAB-5933-4794-945B-E1924D323928}">
   <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -23191,28 +23194,28 @@
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="7" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -23222,29 +23225,29 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -23310,14 +23313,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -23328,28 +23331,28 @@
       <c r="A3" s="95"/>
       <c r="B3" s="95"/>
       <c r="C3" s="22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
@@ -23368,34 +23371,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -23404,7 +23407,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="34">
         <v>7</v>
@@ -23518,7 +23521,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="49">
         <v>17</v>
@@ -23632,7 +23635,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="50">
@@ -23742,7 +23745,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="49">
         <v>19</v>
@@ -23856,7 +23859,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="49">
         <v>16</v>
@@ -23968,7 +23971,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="49">
         <v>13</v>
@@ -24082,7 +24085,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="49">
         <v>14</v>
@@ -24196,7 +24199,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="49"/>
       <c r="D11" s="50">
@@ -24308,7 +24311,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="49">
         <v>20</v>
@@ -24422,7 +24425,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="49">
         <v>18</v>
@@ -24536,7 +24539,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="49">
         <v>12</v>
@@ -24650,7 +24653,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="49">
         <v>13</v>
@@ -24762,7 +24765,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="49">
         <v>13</v>
@@ -24876,7 +24879,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="49">
         <v>8</v>
@@ -24990,7 +24993,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="49">
         <v>7.5</v>
@@ -25104,7 +25107,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="49">
         <v>16.5</v>
@@ -26289,7 +26292,7 @@
     </row>
     <row r="31" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59">
         <f t="shared" ref="C31:J31" si="21">AVERAGE(C4:C19)</f>
@@ -26382,19 +26385,19 @@
     </row>
     <row r="33" spans="18:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R33" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S33" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="T33" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="V33" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -26433,10 +26436,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D17D64C-0221-4B97-86AC-B3E2E90CB6D2}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
@@ -26455,74 +26458,74 @@
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="7" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -26602,14 +26605,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -26620,49 +26623,49 @@
       <c r="A3" s="95"/>
       <c r="B3" s="95"/>
       <c r="C3" s="22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="R3" s="25"/>
       <c r="S3" s="25"/>
@@ -26674,34 +26677,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
@@ -26710,7 +26713,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="34">
         <v>5.5</v>
@@ -26838,7 +26841,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="49">
         <v>8</v>
@@ -26966,7 +26969,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="49">
         <v>7</v>
@@ -27086,7 +27089,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="49">
         <v>2</v>
@@ -27214,7 +27217,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="49">
         <v>5.5</v>
@@ -27342,7 +27345,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="49">
         <v>5</v>
@@ -27470,7 +27473,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="49">
         <v>6</v>
@@ -27598,7 +27601,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="49">
         <v>5.5</v>
@@ -27724,7 +27727,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="49">
         <v>8</v>
@@ -27850,7 +27853,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="49">
         <v>7</v>
@@ -27976,7 +27979,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="49">
         <v>4</v>
@@ -28102,7 +28105,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="49">
         <v>7</v>
@@ -28228,7 +28231,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="49">
         <v>4.5</v>
@@ -28354,7 +28357,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="49">
         <v>5.5</v>
@@ -28478,7 +28481,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="49">
         <v>5</v>
@@ -28602,7 +28605,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="49">
         <v>6.5</v>
@@ -28719,7 +28722,7 @@
     </row>
     <row r="20" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C20" s="59">
         <f t="shared" ref="C20:X20" si="19">AVERAGE(C4:C19)</f>
@@ -28812,19 +28815,19 @@
     </row>
     <row r="22" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R22" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S22" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="T22" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U22" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="V22" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -28864,7 +28867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE4C224D-4664-438B-813E-EAF6B2661C1B}">
   <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -28893,16 +28896,16 @@
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="7" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -28916,29 +28919,29 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -28996,14 +28999,14 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="96" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
       <c r="AE2" s="96"/>
       <c r="AF2" s="97" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="97"/>
       <c r="AH2" s="97"/>
@@ -29014,16 +29017,16 @@
       <c r="A3" s="95"/>
       <c r="B3" s="95"/>
       <c r="C3" s="22" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -29046,34 +29049,34 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="29" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AG3" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -29082,7 +29085,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>Nom!B4</f>
-        <v>Jade</v>
+        <v>A</v>
       </c>
       <c r="C4" s="34">
         <v>14</v>
@@ -29188,7 +29191,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>Nom!B5</f>
-        <v>Emilien</v>
+        <v>B</v>
       </c>
       <c r="C5" s="49">
         <v>16</v>
@@ -29294,7 +29297,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Nom!B6</f>
-        <v>Logan</v>
+        <v>C</v>
       </c>
       <c r="C6" s="49">
         <v>21</v>
@@ -29400,7 +29403,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>Nom!B7</f>
-        <v>Michael</v>
+        <v>D</v>
       </c>
       <c r="C7" s="49">
         <v>20</v>
@@ -29506,7 +29509,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>Nom!B8</f>
-        <v>Asenga</v>
+        <v>E</v>
       </c>
       <c r="C8" s="49">
         <v>22</v>
@@ -29612,7 +29615,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>Nom!B9</f>
-        <v>Angélina</v>
+        <v>F</v>
       </c>
       <c r="C9" s="49">
         <v>15</v>
@@ -29718,7 +29721,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>Nom!B10</f>
-        <v>Henry</v>
+        <v>G</v>
       </c>
       <c r="C10" s="49">
         <v>21</v>
@@ -29824,7 +29827,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>Nom!B11</f>
-        <v>Isalyne</v>
+        <v>H</v>
       </c>
       <c r="C11" s="49">
         <v>16</v>
@@ -29930,7 +29933,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Nom!B12</f>
-        <v>Laura</v>
+        <v>I</v>
       </c>
       <c r="C12" s="49">
         <v>28</v>
@@ -30036,7 +30039,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>Nom!B13</f>
-        <v>Chloé</v>
+        <v>J</v>
       </c>
       <c r="C13" s="49">
         <v>24</v>
@@ -30142,7 +30145,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>Nom!B14</f>
-        <v>Hérésia</v>
+        <v>K</v>
       </c>
       <c r="C14" s="49">
         <v>16</v>
@@ -30248,7 +30251,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>Nom!B15</f>
-        <v>Keurtys</v>
+        <v>L</v>
       </c>
       <c r="C15" s="49">
         <v>20</v>
@@ -30354,7 +30357,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>Nom!B16</f>
-        <v>Clhéo</v>
+        <v>M</v>
       </c>
       <c r="C16" s="49">
         <v>24</v>
@@ -30460,7 +30463,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>Nom!B17</f>
-        <v>Camille</v>
+        <v>N</v>
       </c>
       <c r="C17" s="49">
         <v>11</v>
@@ -30566,7 +30569,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>Nom!B18</f>
-        <v>Emma</v>
+        <v>O</v>
       </c>
       <c r="C18" s="49">
         <v>18</v>
@@ -30672,7 +30675,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>Nom!B19</f>
-        <v>Basile</v>
+        <v>P</v>
       </c>
       <c r="C19" s="49">
         <v>22</v>
@@ -31851,7 +31854,7 @@
     </row>
     <row r="31" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="59">
         <f>AVERAGE(C4:C19)</f>
@@ -31944,19 +31947,19 @@
     </row>
     <row r="33" spans="18:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R33" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S33" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="T33" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="V33" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>